<commit_message>
Agent Commission Setup completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Users.xlsx
+++ b/src/test/resources/testdata/Users.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FD9F0D-4382-44AE-9D69-4B2547704C0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047F2004-4FFE-4EEA-986B-EE14896CEF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{08AC821B-A7C7-4688-B729-8F9B897E42FE}"/>
   </bookViews>
   <sheets>
     <sheet name="ProducerCode" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>AG1730A1</t>
-  </si>
-  <si>
-    <t>AG8160A1</t>
+    <t>AG6304A44</t>
   </si>
 </sst>
 </file>
@@ -54,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +59,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,7 +117,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -114,7 +129,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -161,6 +176,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -196,6 +228,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -347,26 +396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49644198-7EA3-49C5-97BA-3B4AD2B9274B}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after regression updates added. MTR-167 added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Users.xlsx
+++ b/src/test/resources/testdata/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047F2004-4FFE-4EEA-986B-EE14896CEF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFCF9AB-911C-4560-9CCB-ECE744693735}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{08AC821B-A7C7-4688-B729-8F9B897E42FE}"/>
   </bookViews>
@@ -25,9 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>AG6304A44</t>
+    <t>AG6304A74</t>
+  </si>
+  <si>
+    <t>AG6304A47</t>
+  </si>
+  <si>
+    <t>AG6304A79</t>
+  </si>
+  <si>
+    <t>AG6304A100</t>
+  </si>
+  <si>
+    <t>AG6304A117</t>
   </si>
 </sst>
 </file>
@@ -397,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49644198-7EA3-49C5-97BA-3B4AD2B9274B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,6 +425,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MTR-462 and MTR 463 updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Users.xlsx
+++ b/src/test/resources/testdata/Users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcemek\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047F2004-4FFE-4EEA-986B-EE14896CEF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23853828-D5BD-454B-A18A-93AA17B7C478}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{08AC821B-A7C7-4688-B729-8F9B897E42FE}"/>
   </bookViews>
@@ -25,9 +25,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>AG6304A44</t>
+  </si>
+  <si>
+    <t>AG6304A136</t>
+  </si>
+  <si>
+    <t>AG6304A129</t>
+  </si>
+  <si>
+    <t>AG6304A85</t>
+  </si>
+  <si>
+    <t>AG6304A140</t>
+  </si>
+  <si>
+    <t>AG6304A106</t>
+  </si>
+  <si>
+    <t>AG8258A1</t>
+  </si>
+  <si>
+    <t>AG6304A36</t>
+  </si>
+  <si>
+    <t>AG6304A109</t>
+  </si>
+  <si>
+    <t>AG6304A38</t>
+  </si>
+  <si>
+    <t>AG6304A125</t>
+  </si>
+  <si>
+    <t>AG6304A70</t>
+  </si>
+  <si>
+    <t>AG6304A55</t>
+  </si>
+  <si>
+    <t>AG6304A49</t>
+  </si>
+  <si>
+    <t>AG6304A143</t>
+  </si>
+  <si>
+    <t>AG6304A133</t>
+  </si>
+  <si>
+    <t>AG6304A29</t>
+  </si>
+  <si>
+    <t>AG6304A112</t>
+  </si>
+  <si>
+    <t>AG6304A132</t>
+  </si>
+  <si>
+    <t>AG6304A35</t>
+  </si>
+  <si>
+    <t>AG6304A116</t>
+  </si>
+  <si>
+    <t>AG6304A51</t>
+  </si>
+  <si>
+    <t>AG6304A91</t>
   </si>
 </sst>
 </file>
@@ -397,19 +463,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49644198-7EA3-49C5-97BA-3B4AD2B9274B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>